<commit_message>
Completed Finished Goods Report - for checking Updated Misc Report - for rechecking
</commit_message>
<xml_diff>
--- a/ERPReports/ERPReports/Areas/Reports/Templates/LSP_Rpt_DM_MiscellaneousTransactionReport_LSPI.xlsx
+++ b/ERPReports/ERPReports/Areas/Reports/Templates/LSP_Rpt_DM_MiscellaneousTransactionReport_LSPI.xlsx
@@ -4,23 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="135" windowWidth="16140" windowHeight="9990" activeTab="4"/>
+    <workbookView xWindow="285" yWindow="135" windowWidth="16140" windowHeight="9990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="MiscellaneousTransactions" sheetId="7" r:id="rId2"/>
-    <sheet name="Cycle Count" sheetId="2" r:id="rId3"/>
-    <sheet name="Miscellaneous Issue" sheetId="3" r:id="rId4"/>
-    <sheet name="Miscellaneous Receipt" sheetId="4" r:id="rId5"/>
-    <sheet name="SF Scrap Summary" sheetId="5" r:id="rId6"/>
-    <sheet name="SF Scrap Data" sheetId="6" r:id="rId7"/>
+    <sheet name="Cycle Count" sheetId="2" r:id="rId2"/>
+    <sheet name="Miscellaneous Issue" sheetId="3" r:id="rId3"/>
+    <sheet name="Miscellaneous Receipt" sheetId="4" r:id="rId4"/>
+    <sheet name="SF Scrap Summary" sheetId="5" r:id="rId5"/>
+    <sheet name="SF Scrap Data" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'SF Scrap Data'!$A$5:$O$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="4">'Miscellaneous Receipt'!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">MiscellaneousTransactions!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'SF Scrap Data'!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="5">'SF Scrap Summary'!$1:$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'SF Scrap Data'!$A$5:$O$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Miscellaneous Receipt'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'SF Scrap Data'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'SF Scrap Summary'!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Summary!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="27">
   <si>
     <r>
       <t xml:space="preserve">TOTAL COST
@@ -1303,175 +1301,10 @@
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="B37" sqref="B37"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="22.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-    </row>
-    <row r="2" spans="1:13" ht="22.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-    </row>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="13"/>
-    </row>
-    <row r="4" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="9"/>
-    </row>
-    <row r="6" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" ht="409.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G6:L6"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="G3:L3"/>
-  </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.65000000000000013" bottom="0.23" header="0.65000000000000013" footer="0.23"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;C&amp;R</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
-  <dimension ref="A1:M7"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection activeCell="B37" sqref="B37"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1628,7 +1461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -1795,17 +1628,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="C13" sqref="C13"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1960,7 +1793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -2196,7 +2029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>

</xml_diff>

<commit_message>
MiscTrans and RM Breakdown
Update template in Misc. Transaction Report
Stored procedure draft for RM breakdown of FG Report
</commit_message>
<xml_diff>
--- a/ERPReports/ERPReports/Areas/Reports/Templates/LSP_Rpt_DM_MiscellaneousTransactionReport_LSPI.xlsx
+++ b/ERPReports/ERPReports/Areas/Reports/Templates/LSP_Rpt_DM_MiscellaneousTransactionReport_LSPI.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1306E347-B13E-4F91-BC21-F128C0F1E38A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="135" windowWidth="16140" windowHeight="9990" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="MiscellaneousTransactions" sheetId="7" r:id="rId2"/>
-    <sheet name="Cycle Count" sheetId="2" r:id="rId3"/>
-    <sheet name="Miscellaneous Issue" sheetId="3" r:id="rId4"/>
-    <sheet name="Miscellaneous Receipt" sheetId="4" r:id="rId5"/>
-    <sheet name="SF Scrap Summary" sheetId="5" r:id="rId6"/>
-    <sheet name="SF Scrap Data" sheetId="6" r:id="rId7"/>
+    <sheet name="Cycle Count" sheetId="2" r:id="rId2"/>
+    <sheet name="Miscellaneous Issue" sheetId="3" r:id="rId3"/>
+    <sheet name="Miscellaneous Receipt" sheetId="4" r:id="rId4"/>
+    <sheet name="SF Scrap Summary" sheetId="5" r:id="rId5"/>
+    <sheet name="SF Scrap Data" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'SF Scrap Data'!$A$5:$O$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="4">'Miscellaneous Receipt'!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">MiscellaneousTransactions!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'SF Scrap Data'!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="5">'SF Scrap Summary'!$1:$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'SF Scrap Data'!$A$5:$O$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Miscellaneous Receipt'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'SF Scrap Data'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'SF Scrap Summary'!$1:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Summary!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="27">
   <si>
     <r>
       <t xml:space="preserve">TOTAL COST
@@ -140,7 +139,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-10409]m/d/yyyy\ h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-10409]#,##0.00;\(#,##0.00\)"/>
@@ -892,6 +891,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1188,12 +1190,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1297,181 +1299,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection activeCell="B37" sqref="B37"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="22.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-    </row>
-    <row r="2" spans="1:13" ht="22.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-    </row>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="13"/>
-    </row>
-    <row r="4" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="9"/>
-    </row>
-    <row r="6" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" ht="409.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G6:L6"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="G3:L3"/>
-  </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.65000000000000013" bottom="0.23" header="0.65000000000000013" footer="0.23"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;C&amp;R</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
-  <dimension ref="A1:M7"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection activeCell="B37" sqref="B37"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1628,17 +1462,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection activeCell="B37" sqref="B37"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1795,17 +1626,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection activeCell="C13" sqref="C13"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1960,8 +1788,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2196,8 +2024,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>